<commit_message>
fix: evaluation result issue in .csv file.
</commit_message>
<xml_diff>
--- a/src/evaluation_output/input_data.xlsx
+++ b/src/evaluation_output/input_data.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu-22.04\home\jerryhung\scamshield-ai\mock_data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu-22.04\home\jerryhung\scamshield-ai\src\evaluation_output\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -1501,31 +1501,6 @@
 這次的經歷讓我付出了慘痛的代價，也讓我明白，網路上的陌生人，無論看起來多麼友善或可信，都不能輕信，更不要捲入這類可疑的交易。希望我的案例能提醒大家，保持警覺，遠離誘惑，以免落入這些騙局的陷阱！</t>
   </si>
   <si>
-    <t xml:space="preserve">
-[
-  {
-    "id": "13-4色情應召詐財詐騙:約定見面、援交",
-    "label": "色情應召詐財詐騙:約定見面、援交",
-    "evidence": "後來，他邀請我加入他的LINE，ID是「nameiuu」。一開始的對話還挺正常，直到他提到有「兼職援交」的機會，說只要付出一點時間，就能賺到不錯的收入。"
-  },
-  {
-    "id": "13-11色情應召詐財詐騙:需繳保證金給經理才能見面",
-    "label": "色情應召詐財詐騙:需繳保證金給經理才能見面",
-    "evidence": "他聲稱「為了確保雙方的安全和信任」，需要我進行身分確認並繳交保證金。他的說法看起來十分合理，還強調這筆錢會在見面時全額退還。"
-  },
-  {
-    "id": "13-16色情應召詐財詐騙:要求購買遊戲點數後拍照回傳",
-    "label": "色情應召詐財詐騙:要求購買遊戲點數後拍照回傳",
-    "evidence": "於是，我依照他的指示，購買了APPLE STORE點數卡，拍下照片並傳給他。"
-  },
-  {
-    "id": "13-17色情應召詐財詐騙:購買App Store點數卡",
-    "label": "色情應召詐財詐騙:購買App Store點數卡",
-    "evidence": "於是，我依照他的指示，購買了APPLE STORE點數卡，拍下照片並傳給他。"
-  }
-]</t>
-  </si>
-  <si>
     <t>我於113年12月06日在通訊軟體Instagram收到一位暱稱叫阿海的訊息，對方自稱是男模酒店員工，主動邀請我見面，但他說見面錢要支付對方新台幣1萬元才能與他見面，我在12月09日11時32分在7-11超商內購買APP STORE點數1,000點，將點數序號拍照傳給對方，對方又叫我要再湊新台幣9,000元出來，我跟他說沒有辦法，他就說一些威脅的話術嚇我，當下我覺得怪怪的，到派出所請警察協助，才知道我被騙了。</t>
   </si>
   <si>
@@ -3786,32 +3761,6 @@
     <t xml:space="preserve">
 [
   {
-    "id": "13-4色情應召詐財詐騙:約定見面、援交",
-    "label": "色情應召詐財詐騙:約定見面、援交",
-    "evidence": "後來，他邀請我加入他的LINE，ID是「nameiuu」。一開始的對話還挺正常，直到他提到有「兼職援交」的機會，說只要付出一點時間，就能賺到不錯的收入。"
-  },
-  {
-    "id": "13-11色情應召詐財詐騙:需繳保證金給經理才能見面",
-    "label": "色情應召詐財詐騙:需繳保證金給經理才能見面",
-    "evidence": "他聲稱「為了確保雙方的安全和信任」，需要我進行身分確認並繳交保證金。他的說法看起來十分合理，還強調這筆錢會在見面時全額退還。"
-  },
-  {
-    "id": "13-16色情應召詐財詐騙:要求購買遊戲點數後拍照回傳",
-    "label": "色情應召詐財詐騙:要求購買遊戲點數後拍照回傳",
-    "evidence": "於是，我依照他的指示，購買了APPLE STORE點數卡，拍下照片並傳給他。"
-  },
-  {
-    "id": "13-17色情應召詐財詐騙:購買App Store點數卡",
-    "label": "色情應召詐財詐騙:購買App Store點數卡",
-    "evidence": "於是，我依照他的指示，購買了APPLE STORE點數卡，拍下照片並傳給他。"
-  }
-]
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">
-[
-  {
     "id": "13-3",
     "label": "色情應召詐財詐騙:酒店男模",
     "evidence": "對方自稱是男模酒店員工，主動邀請我見面，但他說見面錢要支付對方新台幣1萬元才能與他見面"
@@ -5821,6 +5770,59 @@
   }
 ]
 </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">
+[
+  {
+    "id": "13-4",
+    "label": "色情應召詐財詐騙:約定見面、援交",
+    "evidence": "後來，他邀請我加入他的LINE，ID是「nameiuu」。一開始的對話還挺正常，直到他提到有「兼職援交」的機會，說只要付出一點時間，就能賺到不錯的收入。"
+  },
+  {
+    "id": "13-11",
+    "label": "色情應召詐財詐騙:需繳保證金給經理才能見面",
+    "evidence": "他聲稱「為了確保雙方的安全和信任」，需要我進行身分確認並繳交保證金。他的說法看起來十分合理，還強調這筆錢會在見面時全額退還。"
+  },
+  {
+    "id": "13-16",
+    "label": "色情應召詐財詐騙:要求購買遊戲點數後拍照回傳",
+    "evidence": "於是，我依照他的指示，購買了APPLE STORE點數卡，拍下照片並傳給他。"
+  },
+  {
+    "id": "13-17",
+    "label": "色情應召詐財詐騙:購買App Store點數卡",
+    "evidence": "於是，我依照他的指示，購買了APPLE STORE點數卡，拍下照片並傳給他。"
+  }
+]
+</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">
+[
+  {
+    "id": "13-4",
+    "label": "色情應召詐財詐騙:約定見面、援交",
+    "evidence": "後來，他邀請我加入他的LINE，ID是「nameiuu」。一開始的對話還挺正常，直到他提到有「兼職援交」的機會，說只要付出一點時間，就能賺到不錯的收入。"
+  },
+  {
+    "id": "13-11",
+    "label": "色情應召詐財詐騙:需繳保證金給經理才能見面",
+    "evidence": "他聲稱「為了確保雙方的安全和信任」，需要我進行身分確認並繳交保證金。他的說法看起來十分合理，還強調這筆錢會在見面時全額退還。"
+  },
+  {
+    "id": "13-16",
+    "label": "色情應召詐財詐騙:要求購買遊戲點數後拍照回傳",
+    "evidence": "於是，我依照他的指示，購買了APPLE STORE點數卡，拍下照片並傳給他。"
+  },
+  {
+    "id": "13-17",
+    "label": "色情應召詐財詐騙:購買App Store點數卡",
+    "evidence": "於是，我依照他的指示，購買了APPLE STORE點數卡，拍下照片並傳給他。"
+  }
+]</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -6283,2433 +6285,2433 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" s="8" t="s">
+        <v>284</v>
+      </c>
+      <c r="B1" s="8" t="s">
+        <v>285</v>
+      </c>
+      <c r="C1" s="8" t="s">
         <v>286</v>
-      </c>
-      <c r="B1" s="8" t="s">
-        <v>287</v>
-      </c>
-      <c r="C1" s="8" t="s">
-        <v>288</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" s="7" t="s">
-        <v>415</v>
+        <v>413</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="C2" s="6" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" s="7" t="s">
-        <v>366</v>
+        <v>364</v>
       </c>
       <c r="B3" s="6" t="s">
+        <v>287</v>
+      </c>
+      <c r="C3" s="6" t="s">
         <v>289</v>
-      </c>
-      <c r="C3" s="6" t="s">
-        <v>291</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" s="7" t="s">
-        <v>367</v>
+        <v>365</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="C4" s="6" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" s="7" t="s">
-        <v>368</v>
+        <v>366</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="C5" s="6" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" s="7" t="s">
-        <v>369</v>
+        <v>367</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="C6" s="6" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" s="7" t="s">
-        <v>370</v>
+        <v>368</v>
       </c>
       <c r="B7" s="6" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="C7" s="6" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" s="7" t="s">
-        <v>371</v>
+        <v>369</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="C8" s="6" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" s="7" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
       <c r="B9" s="6" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="C9" s="6" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" s="7" t="s">
-        <v>373</v>
+        <v>371</v>
       </c>
       <c r="B10" s="6" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="C10" s="6" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11" s="7" t="s">
-        <v>374</v>
+        <v>372</v>
       </c>
       <c r="B11" s="6" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="C11" s="6" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12" s="7" t="s">
-        <v>375</v>
+        <v>373</v>
       </c>
       <c r="B12" s="6" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="C12" s="6" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13" s="7" t="s">
-        <v>376</v>
+        <v>374</v>
       </c>
       <c r="B13" s="6" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="C13" s="6" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A14" s="7" t="s">
-        <v>377</v>
+        <v>375</v>
       </c>
       <c r="B14" s="6" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="C14" s="6" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A15" s="7" t="s">
-        <v>378</v>
+        <v>376</v>
       </c>
       <c r="B15" s="6" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="C15" s="6" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A16" s="7" t="s">
-        <v>379</v>
+        <v>377</v>
       </c>
       <c r="B16" s="6" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="C16" s="6" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A17" s="7" t="s">
-        <v>380</v>
+        <v>378</v>
       </c>
       <c r="B17" s="6" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="C17" s="6" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A18" s="7" t="s">
-        <v>381</v>
+        <v>379</v>
       </c>
       <c r="B18" s="6" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="C18" s="6" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A19" s="7" t="s">
-        <v>382</v>
+        <v>380</v>
       </c>
       <c r="B19" s="6" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="C19" s="6" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A20" s="7" t="s">
-        <v>416</v>
+        <v>414</v>
       </c>
       <c r="B20" s="6" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
       <c r="C20" s="6" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A21" s="7" t="s">
-        <v>383</v>
+        <v>381</v>
       </c>
       <c r="B21" s="6" t="s">
+        <v>306</v>
+      </c>
+      <c r="C21" s="6" t="s">
         <v>308</v>
-      </c>
-      <c r="C21" s="6" t="s">
-        <v>310</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A22" s="7" t="s">
-        <v>384</v>
+        <v>382</v>
       </c>
       <c r="B22" s="6" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
       <c r="C22" s="6" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A23" s="7" t="s">
-        <v>385</v>
+        <v>383</v>
       </c>
       <c r="B23" s="6" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
       <c r="C23" s="6" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A24" s="7" t="s">
-        <v>386</v>
+        <v>384</v>
       </c>
       <c r="B24" s="6" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
       <c r="C24" s="6" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A25" s="7" t="s">
-        <v>387</v>
+        <v>385</v>
       </c>
       <c r="B25" s="6" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
       <c r="C25" s="6" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A26" s="7" t="s">
-        <v>388</v>
+        <v>386</v>
       </c>
       <c r="B26" s="6" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
       <c r="C26" s="6" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A27" s="7" t="s">
-        <v>389</v>
+        <v>387</v>
       </c>
       <c r="B27" s="6" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
       <c r="C27" s="6" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A28" s="7" t="s">
-        <v>390</v>
+        <v>388</v>
       </c>
       <c r="B28" s="6" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
       <c r="C28" s="6" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A29" s="7" t="s">
-        <v>391</v>
+        <v>389</v>
       </c>
       <c r="B29" s="6" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
       <c r="C29" s="6" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A30" s="7" t="s">
-        <v>392</v>
+        <v>390</v>
       </c>
       <c r="B30" s="6" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
       <c r="C30" s="6" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A31" s="7" t="s">
-        <v>393</v>
+        <v>391</v>
       </c>
       <c r="B31" s="6" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
       <c r="C31" s="6" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A32" s="7" t="s">
-        <v>394</v>
+        <v>392</v>
       </c>
       <c r="B32" s="6" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
       <c r="C32" s="6" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A33" s="7" t="s">
-        <v>395</v>
+        <v>393</v>
       </c>
       <c r="B33" s="6" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
       <c r="C33" s="6" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A34" s="7" t="s">
-        <v>396</v>
+        <v>394</v>
       </c>
       <c r="B34" s="6" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
       <c r="C34" s="6" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A35" s="7" t="s">
-        <v>417</v>
+        <v>415</v>
       </c>
       <c r="B35" s="6" t="s">
-        <v>324</v>
+        <v>322</v>
       </c>
       <c r="C35" s="6" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A36" s="7" t="s">
-        <v>397</v>
+        <v>395</v>
       </c>
       <c r="B36" s="6" t="s">
+        <v>322</v>
+      </c>
+      <c r="C36" s="6" t="s">
         <v>324</v>
-      </c>
-      <c r="C36" s="6" t="s">
-        <v>326</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A37" s="7" t="s">
-        <v>398</v>
+        <v>396</v>
       </c>
       <c r="B37" s="6" t="s">
-        <v>324</v>
+        <v>322</v>
       </c>
       <c r="C37" s="6" t="s">
-        <v>327</v>
+        <v>325</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A38" s="7" t="s">
-        <v>399</v>
+        <v>397</v>
       </c>
       <c r="B38" s="6" t="s">
-        <v>324</v>
+        <v>322</v>
       </c>
       <c r="C38" s="6" t="s">
-        <v>328</v>
+        <v>326</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A39" s="7" t="s">
-        <v>400</v>
+        <v>398</v>
       </c>
       <c r="B39" s="6" t="s">
-        <v>324</v>
+        <v>322</v>
       </c>
       <c r="C39" s="6" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A40" s="7" t="s">
-        <v>401</v>
+        <v>399</v>
       </c>
       <c r="B40" s="6" t="s">
-        <v>324</v>
+        <v>322</v>
       </c>
       <c r="C40" s="6" t="s">
-        <v>330</v>
+        <v>328</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A41" s="7" t="s">
-        <v>402</v>
+        <v>400</v>
       </c>
       <c r="B41" s="6" t="s">
-        <v>324</v>
+        <v>322</v>
       </c>
       <c r="C41" s="6" t="s">
-        <v>331</v>
+        <v>329</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A42" s="7" t="s">
-        <v>403</v>
+        <v>401</v>
       </c>
       <c r="B42" s="6" t="s">
-        <v>324</v>
+        <v>322</v>
       </c>
       <c r="C42" s="6" t="s">
-        <v>332</v>
+        <v>330</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A43" s="7" t="s">
-        <v>404</v>
+        <v>402</v>
       </c>
       <c r="B43" s="6" t="s">
-        <v>324</v>
+        <v>322</v>
       </c>
       <c r="C43" s="6" t="s">
-        <v>333</v>
+        <v>331</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A44" s="7" t="s">
-        <v>405</v>
+        <v>403</v>
       </c>
       <c r="B44" s="6" t="s">
-        <v>324</v>
+        <v>322</v>
       </c>
       <c r="C44" s="6" t="s">
-        <v>334</v>
+        <v>332</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A45" s="7" t="s">
-        <v>406</v>
+        <v>404</v>
       </c>
       <c r="B45" s="6" t="s">
-        <v>324</v>
+        <v>322</v>
       </c>
       <c r="C45" s="6" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A46" s="7" t="s">
-        <v>407</v>
+        <v>405</v>
       </c>
       <c r="B46" s="6" t="s">
-        <v>324</v>
+        <v>322</v>
       </c>
       <c r="C46" s="6" t="s">
-        <v>336</v>
+        <v>334</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A47" s="7" t="s">
-        <v>408</v>
+        <v>406</v>
       </c>
       <c r="B47" s="6" t="s">
-        <v>324</v>
+        <v>322</v>
       </c>
       <c r="C47" s="6" t="s">
-        <v>337</v>
+        <v>335</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A48" s="7" t="s">
-        <v>409</v>
+        <v>407</v>
       </c>
       <c r="B48" s="6" t="s">
-        <v>324</v>
+        <v>322</v>
       </c>
       <c r="C48" s="6" t="s">
-        <v>338</v>
+        <v>336</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A49" s="7" t="s">
-        <v>410</v>
+        <v>408</v>
       </c>
       <c r="B49" s="6" t="s">
-        <v>324</v>
+        <v>322</v>
       </c>
       <c r="C49" s="6" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A50" s="7" t="s">
-        <v>411</v>
+        <v>409</v>
       </c>
       <c r="B50" s="6" t="s">
-        <v>324</v>
+        <v>322</v>
       </c>
       <c r="C50" s="6" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A51" s="7" t="s">
-        <v>412</v>
+        <v>410</v>
       </c>
       <c r="B51" s="6" t="s">
-        <v>324</v>
+        <v>322</v>
       </c>
       <c r="C51" s="6" t="s">
-        <v>341</v>
+        <v>339</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A52" s="7" t="s">
-        <v>413</v>
+        <v>411</v>
       </c>
       <c r="B52" s="6" t="s">
-        <v>324</v>
+        <v>322</v>
       </c>
       <c r="C52" s="6" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A53" s="7" t="s">
-        <v>414</v>
+        <v>412</v>
       </c>
       <c r="B53" s="6" t="s">
-        <v>324</v>
+        <v>322</v>
       </c>
       <c r="C53" s="6" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A54" s="7" t="s">
-        <v>418</v>
+        <v>416</v>
       </c>
       <c r="B54" s="6" t="s">
-        <v>324</v>
+        <v>322</v>
       </c>
       <c r="C54" s="6" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A55" s="7" t="s">
-        <v>419</v>
+        <v>417</v>
       </c>
       <c r="B55" s="6" t="s">
-        <v>345</v>
+        <v>343</v>
       </c>
       <c r="C55" s="6" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A56" s="7" t="s">
-        <v>420</v>
+        <v>418</v>
       </c>
       <c r="B56" s="6" t="s">
+        <v>343</v>
+      </c>
+      <c r="C56" s="6" t="s">
         <v>345</v>
-      </c>
-      <c r="C56" s="6" t="s">
-        <v>347</v>
       </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A57" s="7" t="s">
-        <v>421</v>
+        <v>419</v>
       </c>
       <c r="B57" s="6" t="s">
-        <v>345</v>
+        <v>343</v>
       </c>
       <c r="C57" s="6" t="s">
-        <v>348</v>
+        <v>346</v>
       </c>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A58" s="7" t="s">
-        <v>422</v>
+        <v>420</v>
       </c>
       <c r="B58" s="6" t="s">
-        <v>345</v>
+        <v>343</v>
       </c>
       <c r="C58" s="6" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A59" s="7" t="s">
-        <v>423</v>
+        <v>421</v>
       </c>
       <c r="B59" s="6" t="s">
-        <v>345</v>
+        <v>343</v>
       </c>
       <c r="C59" s="6" t="s">
-        <v>350</v>
+        <v>348</v>
       </c>
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A60" s="7" t="s">
-        <v>424</v>
+        <v>422</v>
       </c>
       <c r="B60" s="6" t="s">
-        <v>345</v>
+        <v>343</v>
       </c>
       <c r="C60" s="6" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A61" s="7" t="s">
-        <v>425</v>
+        <v>423</v>
       </c>
       <c r="B61" s="6" t="s">
-        <v>345</v>
+        <v>343</v>
       </c>
       <c r="C61" s="6" t="s">
-        <v>352</v>
+        <v>350</v>
       </c>
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A62" s="7" t="s">
-        <v>426</v>
+        <v>424</v>
       </c>
       <c r="B62" s="6" t="s">
-        <v>345</v>
+        <v>343</v>
       </c>
       <c r="C62" s="6" t="s">
-        <v>353</v>
+        <v>351</v>
       </c>
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A63" s="7" t="s">
-        <v>427</v>
+        <v>425</v>
       </c>
       <c r="B63" s="6" t="s">
-        <v>345</v>
+        <v>343</v>
       </c>
       <c r="C63" s="6" t="s">
-        <v>354</v>
+        <v>352</v>
       </c>
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A64" s="7" t="s">
-        <v>428</v>
+        <v>426</v>
       </c>
       <c r="B64" s="6" t="s">
-        <v>345</v>
+        <v>343</v>
       </c>
       <c r="C64" s="6" t="s">
-        <v>355</v>
+        <v>353</v>
       </c>
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A65" s="7" t="s">
-        <v>429</v>
+        <v>427</v>
       </c>
       <c r="B65" s="6" t="s">
-        <v>345</v>
+        <v>343</v>
       </c>
       <c r="C65" s="6" t="s">
-        <v>356</v>
+        <v>354</v>
       </c>
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A66" s="7" t="s">
-        <v>430</v>
+        <v>428</v>
       </c>
       <c r="B66" s="6" t="s">
-        <v>345</v>
+        <v>343</v>
       </c>
       <c r="C66" s="6" t="s">
-        <v>357</v>
+        <v>355</v>
       </c>
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A67" s="7" t="s">
-        <v>431</v>
+        <v>429</v>
       </c>
       <c r="B67" s="6" t="s">
-        <v>345</v>
+        <v>343</v>
       </c>
       <c r="C67" s="6" t="s">
-        <v>358</v>
+        <v>356</v>
       </c>
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A68" s="7" t="s">
-        <v>432</v>
+        <v>430</v>
       </c>
       <c r="B68" s="6" t="s">
-        <v>345</v>
+        <v>343</v>
       </c>
       <c r="C68" s="6" t="s">
-        <v>359</v>
+        <v>357</v>
       </c>
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A69" s="7" t="s">
-        <v>433</v>
+        <v>431</v>
       </c>
       <c r="B69" s="6" t="s">
-        <v>345</v>
+        <v>343</v>
       </c>
       <c r="C69" s="6" t="s">
-        <v>360</v>
+        <v>358</v>
       </c>
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A70" s="7" t="s">
-        <v>434</v>
+        <v>432</v>
       </c>
       <c r="B70" s="6" t="s">
-        <v>345</v>
+        <v>343</v>
       </c>
       <c r="C70" s="6" t="s">
-        <v>361</v>
+        <v>359</v>
       </c>
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A71" s="7" t="s">
-        <v>435</v>
+        <v>433</v>
       </c>
       <c r="B71" s="6" t="s">
-        <v>345</v>
+        <v>343</v>
       </c>
       <c r="C71" s="6" t="s">
-        <v>362</v>
+        <v>360</v>
       </c>
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A72" s="7" t="s">
-        <v>436</v>
+        <v>434</v>
       </c>
       <c r="B72" s="6" t="s">
-        <v>345</v>
+        <v>343</v>
       </c>
       <c r="C72" s="6" t="s">
-        <v>363</v>
+        <v>361</v>
       </c>
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A73" s="7" t="s">
-        <v>437</v>
+        <v>435</v>
       </c>
       <c r="B73" s="6" t="s">
-        <v>345</v>
+        <v>343</v>
       </c>
       <c r="C73" s="6" t="s">
-        <v>364</v>
+        <v>362</v>
       </c>
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A74" s="7" t="s">
-        <v>438</v>
+        <v>436</v>
       </c>
       <c r="B74" s="6" t="s">
-        <v>345</v>
+        <v>343</v>
       </c>
       <c r="C74" s="6" t="s">
-        <v>365</v>
+        <v>363</v>
       </c>
     </row>
     <row r="75" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A75" s="7" t="s">
+        <v>437</v>
+      </c>
+      <c r="B75" s="6" t="s">
+        <v>438</v>
+      </c>
+      <c r="C75" s="6" t="s">
         <v>439</v>
-      </c>
-      <c r="B75" s="6" t="s">
-        <v>440</v>
-      </c>
-      <c r="C75" s="6" t="s">
-        <v>441</v>
       </c>
     </row>
     <row r="76" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A76" s="7" t="s">
-        <v>442</v>
+        <v>440</v>
       </c>
       <c r="B76" s="6" t="s">
-        <v>440</v>
+        <v>438</v>
       </c>
       <c r="C76" s="6" t="s">
-        <v>443</v>
+        <v>441</v>
       </c>
     </row>
     <row r="77" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A77" s="7" t="s">
-        <v>444</v>
+        <v>442</v>
       </c>
       <c r="B77" s="6" t="s">
-        <v>440</v>
+        <v>438</v>
       </c>
       <c r="C77" s="6" t="s">
-        <v>445</v>
+        <v>443</v>
       </c>
     </row>
     <row r="78" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A78" s="7" t="s">
-        <v>446</v>
+        <v>444</v>
       </c>
       <c r="B78" s="6" t="s">
-        <v>440</v>
+        <v>438</v>
       </c>
       <c r="C78" s="6" t="s">
-        <v>447</v>
+        <v>445</v>
       </c>
     </row>
     <row r="79" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A79" s="7" t="s">
-        <v>448</v>
+        <v>446</v>
       </c>
       <c r="B79" s="6" t="s">
-        <v>440</v>
+        <v>438</v>
       </c>
       <c r="C79" s="6" t="s">
-        <v>449</v>
+        <v>447</v>
       </c>
     </row>
     <row r="80" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A80" s="7" t="s">
-        <v>450</v>
+        <v>448</v>
       </c>
       <c r="B80" s="6" t="s">
-        <v>440</v>
+        <v>438</v>
       </c>
       <c r="C80" s="6" t="s">
-        <v>451</v>
+        <v>449</v>
       </c>
     </row>
     <row r="81" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A81" s="7" t="s">
-        <v>452</v>
+        <v>450</v>
       </c>
       <c r="B81" s="6" t="s">
-        <v>440</v>
+        <v>438</v>
       </c>
       <c r="C81" s="6" t="s">
-        <v>453</v>
+        <v>451</v>
       </c>
     </row>
     <row r="82" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A82" s="7" t="s">
-        <v>454</v>
+        <v>452</v>
       </c>
       <c r="B82" s="6" t="s">
-        <v>440</v>
+        <v>438</v>
       </c>
       <c r="C82" s="6" t="s">
-        <v>455</v>
+        <v>453</v>
       </c>
     </row>
     <row r="83" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A83" s="7" t="s">
-        <v>456</v>
+        <v>454</v>
       </c>
       <c r="B83" s="6" t="s">
-        <v>440</v>
+        <v>438</v>
       </c>
       <c r="C83" s="6" t="s">
-        <v>457</v>
+        <v>455</v>
       </c>
     </row>
     <row r="84" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A84" s="7" t="s">
-        <v>458</v>
+        <v>456</v>
       </c>
       <c r="B84" s="6" t="s">
-        <v>440</v>
+        <v>438</v>
       </c>
       <c r="C84" s="6" t="s">
-        <v>459</v>
+        <v>457</v>
       </c>
     </row>
     <row r="85" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A85" s="7" t="s">
-        <v>460</v>
+        <v>458</v>
       </c>
       <c r="B85" s="6" t="s">
-        <v>440</v>
+        <v>438</v>
       </c>
       <c r="C85" s="6" t="s">
-        <v>461</v>
+        <v>459</v>
       </c>
     </row>
     <row r="86" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A86" s="7" t="s">
-        <v>462</v>
+        <v>460</v>
       </c>
       <c r="B86" s="6" t="s">
-        <v>440</v>
+        <v>438</v>
       </c>
       <c r="C86" s="6" t="s">
-        <v>463</v>
+        <v>461</v>
       </c>
     </row>
     <row r="87" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A87" s="7" t="s">
-        <v>464</v>
+        <v>462</v>
       </c>
       <c r="B87" s="6" t="s">
-        <v>440</v>
+        <v>438</v>
       </c>
       <c r="C87" s="6" t="s">
-        <v>465</v>
+        <v>463</v>
       </c>
     </row>
     <row r="88" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A88" s="7" t="s">
-        <v>466</v>
+        <v>464</v>
       </c>
       <c r="B88" s="6" t="s">
-        <v>440</v>
+        <v>438</v>
       </c>
       <c r="C88" s="6" t="s">
-        <v>467</v>
+        <v>465</v>
       </c>
     </row>
     <row r="89" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A89" s="7" t="s">
-        <v>468</v>
+        <v>466</v>
       </c>
       <c r="B89" s="6" t="s">
-        <v>440</v>
+        <v>438</v>
       </c>
       <c r="C89" s="6" t="s">
-        <v>469</v>
+        <v>467</v>
       </c>
     </row>
     <row r="90" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A90" s="7" t="s">
-        <v>470</v>
+        <v>468</v>
       </c>
       <c r="B90" s="6" t="s">
-        <v>440</v>
+        <v>438</v>
       </c>
       <c r="C90" s="6" t="s">
-        <v>471</v>
+        <v>469</v>
       </c>
     </row>
     <row r="91" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A91" s="7" t="s">
-        <v>472</v>
+        <v>470</v>
       </c>
       <c r="B91" s="6" t="s">
-        <v>440</v>
+        <v>438</v>
       </c>
       <c r="C91" s="6" t="s">
-        <v>473</v>
+        <v>471</v>
       </c>
     </row>
     <row r="92" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A92" s="7" t="s">
-        <v>474</v>
+        <v>472</v>
       </c>
       <c r="B92" s="6" t="s">
-        <v>440</v>
+        <v>438</v>
       </c>
       <c r="C92" s="6" t="s">
-        <v>475</v>
+        <v>473</v>
       </c>
     </row>
     <row r="93" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A93" s="7" t="s">
-        <v>476</v>
+        <v>474</v>
       </c>
       <c r="B93" s="6" t="s">
-        <v>440</v>
+        <v>438</v>
       </c>
       <c r="C93" s="6" t="s">
-        <v>477</v>
+        <v>475</v>
       </c>
     </row>
     <row r="94" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A94" s="7" t="s">
+        <v>476</v>
+      </c>
+      <c r="B94" s="6" t="s">
+        <v>477</v>
+      </c>
+      <c r="C94" s="6" t="s">
         <v>478</v>
-      </c>
-      <c r="B94" s="6" t="s">
-        <v>479</v>
-      </c>
-      <c r="C94" s="6" t="s">
-        <v>480</v>
       </c>
     </row>
     <row r="95" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A95" s="7" t="s">
-        <v>481</v>
+        <v>479</v>
       </c>
       <c r="B95" s="6" t="s">
-        <v>479</v>
+        <v>477</v>
       </c>
       <c r="C95" s="6" t="s">
-        <v>482</v>
+        <v>480</v>
       </c>
     </row>
     <row r="96" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A96" s="7" t="s">
-        <v>483</v>
+        <v>481</v>
       </c>
       <c r="B96" s="6" t="s">
-        <v>479</v>
+        <v>477</v>
       </c>
       <c r="C96" s="6" t="s">
-        <v>484</v>
+        <v>482</v>
       </c>
     </row>
     <row r="97" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A97" s="7" t="s">
-        <v>485</v>
+        <v>483</v>
       </c>
       <c r="B97" s="6" t="s">
-        <v>479</v>
+        <v>477</v>
       </c>
       <c r="C97" s="6" t="s">
-        <v>486</v>
+        <v>484</v>
       </c>
     </row>
     <row r="98" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A98" s="7" t="s">
-        <v>487</v>
+        <v>485</v>
       </c>
       <c r="B98" s="6" t="s">
-        <v>479</v>
+        <v>477</v>
       </c>
       <c r="C98" s="6" t="s">
-        <v>488</v>
+        <v>486</v>
       </c>
     </row>
     <row r="99" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A99" s="7" t="s">
-        <v>489</v>
+        <v>487</v>
       </c>
       <c r="B99" s="6" t="s">
-        <v>479</v>
+        <v>477</v>
       </c>
       <c r="C99" s="6" t="s">
-        <v>490</v>
+        <v>488</v>
       </c>
     </row>
     <row r="100" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A100" s="7" t="s">
-        <v>491</v>
+        <v>489</v>
       </c>
       <c r="B100" s="6" t="s">
-        <v>479</v>
+        <v>477</v>
       </c>
       <c r="C100" s="6" t="s">
-        <v>492</v>
+        <v>490</v>
       </c>
     </row>
     <row r="101" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A101" s="7" t="s">
-        <v>493</v>
+        <v>491</v>
       </c>
       <c r="B101" s="6" t="s">
-        <v>479</v>
+        <v>477</v>
       </c>
       <c r="C101" s="6" t="s">
-        <v>494</v>
+        <v>492</v>
       </c>
     </row>
     <row r="102" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A102" s="7" t="s">
-        <v>495</v>
+        <v>493</v>
       </c>
       <c r="B102" s="6" t="s">
-        <v>479</v>
+        <v>477</v>
       </c>
       <c r="C102" s="6" t="s">
-        <v>496</v>
+        <v>494</v>
       </c>
     </row>
     <row r="103" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A103" s="7" t="s">
-        <v>497</v>
+        <v>495</v>
       </c>
       <c r="B103" s="6" t="s">
-        <v>479</v>
+        <v>477</v>
       </c>
       <c r="C103" s="6" t="s">
-        <v>498</v>
+        <v>496</v>
       </c>
     </row>
     <row r="104" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A104" s="7" t="s">
-        <v>499</v>
+        <v>497</v>
       </c>
       <c r="B104" s="6" t="s">
-        <v>479</v>
+        <v>477</v>
       </c>
       <c r="C104" s="6" t="s">
-        <v>500</v>
+        <v>498</v>
       </c>
     </row>
     <row r="105" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A105" s="7" t="s">
-        <v>501</v>
+        <v>499</v>
       </c>
       <c r="B105" s="6" t="s">
-        <v>479</v>
+        <v>477</v>
       </c>
       <c r="C105" s="6" t="s">
-        <v>502</v>
+        <v>500</v>
       </c>
     </row>
     <row r="106" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A106" s="7" t="s">
-        <v>503</v>
+        <v>501</v>
       </c>
       <c r="B106" s="6" t="s">
-        <v>479</v>
+        <v>477</v>
       </c>
       <c r="C106" s="6" t="s">
-        <v>504</v>
+        <v>502</v>
       </c>
     </row>
     <row r="107" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A107" s="7" t="s">
-        <v>505</v>
+        <v>503</v>
       </c>
       <c r="B107" s="6" t="s">
-        <v>479</v>
+        <v>477</v>
       </c>
       <c r="C107" s="6" t="s">
-        <v>506</v>
+        <v>504</v>
       </c>
     </row>
     <row r="108" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A108" s="7" t="s">
-        <v>507</v>
+        <v>505</v>
       </c>
       <c r="B108" s="6" t="s">
-        <v>479</v>
+        <v>477</v>
       </c>
       <c r="C108" s="6" t="s">
-        <v>508</v>
+        <v>506</v>
       </c>
     </row>
     <row r="109" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A109" s="7" t="s">
-        <v>509</v>
+        <v>507</v>
       </c>
       <c r="B109" s="6" t="s">
-        <v>479</v>
+        <v>477</v>
       </c>
       <c r="C109" s="6" t="s">
-        <v>510</v>
+        <v>508</v>
       </c>
     </row>
     <row r="110" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A110" s="7" t="s">
-        <v>511</v>
+        <v>509</v>
       </c>
       <c r="B110" s="6" t="s">
-        <v>479</v>
+        <v>477</v>
       </c>
       <c r="C110" s="6" t="s">
-        <v>512</v>
+        <v>510</v>
       </c>
     </row>
     <row r="111" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A111" s="7" t="s">
-        <v>513</v>
+        <v>511</v>
       </c>
       <c r="B111" s="6" t="s">
-        <v>479</v>
+        <v>477</v>
       </c>
       <c r="C111" s="6" t="s">
-        <v>514</v>
+        <v>512</v>
       </c>
     </row>
     <row r="112" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A112" s="7" t="s">
-        <v>515</v>
+        <v>513</v>
       </c>
       <c r="B112" s="6" t="s">
-        <v>479</v>
+        <v>477</v>
       </c>
       <c r="C112" s="6" t="s">
-        <v>516</v>
+        <v>514</v>
       </c>
     </row>
     <row r="113" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A113" s="7" t="s">
-        <v>517</v>
+        <v>515</v>
       </c>
       <c r="B113" s="6" t="s">
-        <v>479</v>
+        <v>477</v>
       </c>
       <c r="C113" s="6" t="s">
-        <v>518</v>
+        <v>516</v>
       </c>
     </row>
     <row r="114" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A114" s="7" t="s">
+        <v>517</v>
+      </c>
+      <c r="B114" s="6" t="s">
+        <v>518</v>
+      </c>
+      <c r="C114" s="6" t="s">
         <v>519</v>
-      </c>
-      <c r="B114" s="6" t="s">
-        <v>520</v>
-      </c>
-      <c r="C114" s="6" t="s">
-        <v>521</v>
       </c>
     </row>
     <row r="115" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A115" s="7" t="s">
-        <v>522</v>
+        <v>520</v>
       </c>
       <c r="B115" s="6" t="s">
-        <v>520</v>
+        <v>518</v>
       </c>
       <c r="C115" s="6" t="s">
-        <v>523</v>
+        <v>521</v>
       </c>
     </row>
     <row r="116" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A116" s="7" t="s">
-        <v>524</v>
+        <v>522</v>
       </c>
       <c r="B116" s="6" t="s">
-        <v>520</v>
+        <v>518</v>
       </c>
       <c r="C116" s="6" t="s">
-        <v>525</v>
+        <v>523</v>
       </c>
     </row>
     <row r="117" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A117" s="7" t="s">
-        <v>526</v>
+        <v>524</v>
       </c>
       <c r="B117" s="6" t="s">
-        <v>520</v>
+        <v>518</v>
       </c>
       <c r="C117" s="6" t="s">
-        <v>527</v>
+        <v>525</v>
       </c>
     </row>
     <row r="118" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A118" s="7" t="s">
-        <v>528</v>
+        <v>526</v>
       </c>
       <c r="B118" s="6" t="s">
-        <v>520</v>
+        <v>518</v>
       </c>
       <c r="C118" s="6" t="s">
-        <v>529</v>
+        <v>527</v>
       </c>
     </row>
     <row r="119" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A119" s="7" t="s">
-        <v>530</v>
+        <v>528</v>
       </c>
       <c r="B119" s="6" t="s">
-        <v>520</v>
+        <v>518</v>
       </c>
       <c r="C119" s="6" t="s">
-        <v>531</v>
+        <v>529</v>
       </c>
     </row>
     <row r="120" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A120" s="7" t="s">
-        <v>532</v>
+        <v>530</v>
       </c>
       <c r="B120" s="6" t="s">
-        <v>520</v>
+        <v>518</v>
       </c>
       <c r="C120" s="6" t="s">
-        <v>533</v>
+        <v>531</v>
       </c>
     </row>
     <row r="121" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A121" s="7" t="s">
-        <v>534</v>
+        <v>532</v>
       </c>
       <c r="B121" s="6" t="s">
-        <v>520</v>
+        <v>518</v>
       </c>
       <c r="C121" s="6" t="s">
-        <v>535</v>
+        <v>533</v>
       </c>
     </row>
     <row r="122" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A122" s="7" t="s">
-        <v>536</v>
+        <v>534</v>
       </c>
       <c r="B122" s="6" t="s">
-        <v>520</v>
+        <v>518</v>
       </c>
       <c r="C122" s="6" t="s">
-        <v>537</v>
+        <v>535</v>
       </c>
     </row>
     <row r="123" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A123" s="7" t="s">
-        <v>538</v>
+        <v>536</v>
       </c>
       <c r="B123" s="6" t="s">
-        <v>520</v>
+        <v>518</v>
       </c>
       <c r="C123" s="6" t="s">
-        <v>539</v>
+        <v>537</v>
       </c>
     </row>
     <row r="124" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A124" s="7" t="s">
-        <v>540</v>
+        <v>538</v>
       </c>
       <c r="B124" s="6" t="s">
-        <v>520</v>
+        <v>518</v>
       </c>
       <c r="C124" s="6" t="s">
-        <v>541</v>
+        <v>539</v>
       </c>
     </row>
     <row r="125" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A125" s="7" t="s">
-        <v>542</v>
+        <v>540</v>
       </c>
       <c r="B125" s="6" t="s">
-        <v>520</v>
+        <v>518</v>
       </c>
       <c r="C125" s="6" t="s">
-        <v>543</v>
+        <v>541</v>
       </c>
     </row>
     <row r="126" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A126" s="7" t="s">
-        <v>544</v>
+        <v>542</v>
       </c>
       <c r="B126" s="6" t="s">
-        <v>520</v>
+        <v>518</v>
       </c>
       <c r="C126" s="6" t="s">
-        <v>545</v>
+        <v>543</v>
       </c>
     </row>
     <row r="127" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A127" s="7" t="s">
-        <v>546</v>
+        <v>544</v>
       </c>
       <c r="B127" s="6" t="s">
-        <v>520</v>
+        <v>518</v>
       </c>
       <c r="C127" s="6" t="s">
-        <v>547</v>
+        <v>545</v>
       </c>
     </row>
     <row r="128" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A128" s="7" t="s">
-        <v>548</v>
+        <v>546</v>
       </c>
       <c r="B128" s="6" t="s">
-        <v>520</v>
+        <v>518</v>
       </c>
       <c r="C128" s="6" t="s">
-        <v>549</v>
+        <v>547</v>
       </c>
     </row>
     <row r="129" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A129" s="7" t="s">
-        <v>550</v>
+        <v>548</v>
       </c>
       <c r="B129" s="6" t="s">
-        <v>520</v>
+        <v>518</v>
       </c>
       <c r="C129" s="6" t="s">
-        <v>551</v>
+        <v>549</v>
       </c>
     </row>
     <row r="130" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A130" s="7" t="s">
-        <v>552</v>
+        <v>550</v>
       </c>
       <c r="B130" s="6" t="s">
-        <v>520</v>
+        <v>518</v>
       </c>
       <c r="C130" s="6" t="s">
-        <v>553</v>
+        <v>551</v>
       </c>
     </row>
     <row r="131" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A131" s="7" t="s">
-        <v>554</v>
+        <v>552</v>
       </c>
       <c r="B131" s="6" t="s">
-        <v>520</v>
+        <v>518</v>
       </c>
       <c r="C131" s="6" t="s">
-        <v>555</v>
+        <v>553</v>
       </c>
     </row>
     <row r="132" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A132" s="7" t="s">
-        <v>556</v>
+        <v>554</v>
       </c>
       <c r="B132" s="6" t="s">
-        <v>520</v>
+        <v>518</v>
       </c>
       <c r="C132" s="6" t="s">
-        <v>557</v>
+        <v>555</v>
       </c>
     </row>
     <row r="133" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A133" s="7" t="s">
+        <v>556</v>
+      </c>
+      <c r="B133" s="6" t="s">
+        <v>557</v>
+      </c>
+      <c r="C133" s="6" t="s">
         <v>558</v>
-      </c>
-      <c r="B133" s="6" t="s">
-        <v>559</v>
-      </c>
-      <c r="C133" s="6" t="s">
-        <v>560</v>
       </c>
     </row>
     <row r="134" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A134" s="7" t="s">
-        <v>561</v>
+        <v>559</v>
       </c>
       <c r="B134" s="6" t="s">
-        <v>559</v>
+        <v>557</v>
       </c>
       <c r="C134" s="6" t="s">
-        <v>562</v>
+        <v>560</v>
       </c>
     </row>
     <row r="135" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A135" s="7" t="s">
-        <v>563</v>
+        <v>561</v>
       </c>
       <c r="B135" s="6" t="s">
-        <v>559</v>
+        <v>557</v>
       </c>
       <c r="C135" s="6" t="s">
-        <v>564</v>
+        <v>562</v>
       </c>
     </row>
     <row r="136" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A136" s="7" t="s">
-        <v>565</v>
+        <v>563</v>
       </c>
       <c r="B136" s="6" t="s">
-        <v>559</v>
+        <v>557</v>
       </c>
       <c r="C136" s="6" t="s">
-        <v>566</v>
+        <v>564</v>
       </c>
     </row>
     <row r="137" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A137" s="7" t="s">
+        <v>565</v>
+      </c>
+      <c r="B137" s="6" t="s">
+        <v>566</v>
+      </c>
+      <c r="C137" s="6" t="s">
         <v>567</v>
-      </c>
-      <c r="B137" s="6" t="s">
-        <v>568</v>
-      </c>
-      <c r="C137" s="6" t="s">
-        <v>569</v>
       </c>
     </row>
     <row r="138" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A138" s="7" t="s">
-        <v>570</v>
+        <v>568</v>
       </c>
       <c r="B138" s="6" t="s">
-        <v>568</v>
+        <v>566</v>
       </c>
       <c r="C138" s="6" t="s">
-        <v>571</v>
+        <v>569</v>
       </c>
     </row>
     <row r="139" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A139" s="7" t="s">
-        <v>572</v>
+        <v>570</v>
       </c>
       <c r="B139" s="6" t="s">
-        <v>568</v>
+        <v>566</v>
       </c>
       <c r="C139" s="6" t="s">
-        <v>573</v>
+        <v>571</v>
       </c>
     </row>
     <row r="140" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A140" s="7" t="s">
-        <v>574</v>
+        <v>572</v>
       </c>
       <c r="B140" s="6" t="s">
-        <v>568</v>
+        <v>566</v>
       </c>
       <c r="C140" s="6" t="s">
-        <v>575</v>
+        <v>573</v>
       </c>
     </row>
     <row r="141" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A141" s="7" t="s">
-        <v>576</v>
+        <v>574</v>
       </c>
       <c r="B141" s="6" t="s">
-        <v>568</v>
+        <v>566</v>
       </c>
       <c r="C141" s="6" t="s">
-        <v>577</v>
+        <v>575</v>
       </c>
     </row>
     <row r="142" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A142" s="7" t="s">
-        <v>578</v>
+        <v>576</v>
       </c>
       <c r="B142" s="6" t="s">
-        <v>568</v>
+        <v>566</v>
       </c>
       <c r="C142" s="6" t="s">
-        <v>579</v>
+        <v>577</v>
       </c>
     </row>
     <row r="143" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A143" s="7" t="s">
-        <v>580</v>
+        <v>578</v>
       </c>
       <c r="B143" s="6" t="s">
-        <v>568</v>
+        <v>566</v>
       </c>
       <c r="C143" s="6" t="s">
-        <v>581</v>
+        <v>579</v>
       </c>
     </row>
     <row r="144" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A144" s="7" t="s">
-        <v>582</v>
+        <v>580</v>
       </c>
       <c r="B144" s="6" t="s">
-        <v>568</v>
+        <v>566</v>
       </c>
       <c r="C144" s="6" t="s">
-        <v>583</v>
+        <v>581</v>
       </c>
     </row>
     <row r="145" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A145" s="7" t="s">
-        <v>584</v>
+        <v>582</v>
       </c>
       <c r="B145" s="6" t="s">
-        <v>568</v>
+        <v>566</v>
       </c>
       <c r="C145" s="6" t="s">
-        <v>585</v>
+        <v>583</v>
       </c>
     </row>
     <row r="146" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A146" s="7" t="s">
-        <v>586</v>
+        <v>584</v>
       </c>
       <c r="B146" s="6" t="s">
-        <v>568</v>
+        <v>566</v>
       </c>
       <c r="C146" s="6" t="s">
-        <v>587</v>
+        <v>585</v>
       </c>
     </row>
     <row r="147" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A147" s="7" t="s">
-        <v>588</v>
+        <v>586</v>
       </c>
       <c r="B147" s="6" t="s">
-        <v>568</v>
+        <v>566</v>
       </c>
       <c r="C147" s="6" t="s">
-        <v>589</v>
+        <v>587</v>
       </c>
     </row>
     <row r="148" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A148" s="7" t="s">
-        <v>590</v>
+        <v>588</v>
       </c>
       <c r="B148" s="6" t="s">
-        <v>568</v>
+        <v>566</v>
       </c>
       <c r="C148" s="6" t="s">
-        <v>591</v>
+        <v>589</v>
       </c>
     </row>
     <row r="149" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A149" s="7" t="s">
-        <v>592</v>
+        <v>590</v>
       </c>
       <c r="B149" s="6" t="s">
-        <v>568</v>
+        <v>566</v>
       </c>
       <c r="C149" s="6" t="s">
-        <v>593</v>
+        <v>591</v>
       </c>
     </row>
     <row r="150" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A150" s="7" t="s">
-        <v>594</v>
+        <v>592</v>
       </c>
       <c r="B150" s="6" t="s">
-        <v>568</v>
+        <v>566</v>
       </c>
       <c r="C150" s="6" t="s">
-        <v>595</v>
+        <v>593</v>
       </c>
     </row>
     <row r="151" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A151" s="7" t="s">
-        <v>596</v>
+        <v>594</v>
       </c>
       <c r="B151" s="6" t="s">
-        <v>568</v>
+        <v>566</v>
       </c>
       <c r="C151" s="6" t="s">
-        <v>597</v>
+        <v>595</v>
       </c>
     </row>
     <row r="152" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A152" s="7" t="s">
-        <v>598</v>
+        <v>596</v>
       </c>
       <c r="B152" s="6" t="s">
-        <v>568</v>
+        <v>566</v>
       </c>
       <c r="C152" s="6" t="s">
-        <v>599</v>
+        <v>597</v>
       </c>
     </row>
     <row r="153" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A153" s="7" t="s">
-        <v>600</v>
+        <v>598</v>
       </c>
       <c r="B153" s="6" t="s">
-        <v>568</v>
+        <v>566</v>
       </c>
       <c r="C153" s="6" t="s">
-        <v>601</v>
+        <v>599</v>
       </c>
     </row>
     <row r="154" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A154" s="7" t="s">
-        <v>602</v>
+        <v>600</v>
       </c>
       <c r="B154" s="6" t="s">
-        <v>568</v>
+        <v>566</v>
       </c>
       <c r="C154" s="6" t="s">
-        <v>603</v>
+        <v>601</v>
       </c>
     </row>
     <row r="155" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A155" s="7" t="s">
-        <v>604</v>
+        <v>602</v>
       </c>
       <c r="B155" s="6" t="s">
-        <v>568</v>
+        <v>566</v>
       </c>
       <c r="C155" s="6" t="s">
-        <v>605</v>
+        <v>603</v>
       </c>
     </row>
     <row r="156" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A156" s="7" t="s">
-        <v>606</v>
+        <v>604</v>
       </c>
       <c r="B156" s="6" t="s">
-        <v>568</v>
+        <v>566</v>
       </c>
       <c r="C156" s="6" t="s">
-        <v>607</v>
+        <v>605</v>
       </c>
     </row>
     <row r="157" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A157" s="7" t="s">
-        <v>608</v>
+        <v>606</v>
       </c>
       <c r="B157" s="6" t="s">
-        <v>568</v>
+        <v>566</v>
       </c>
       <c r="C157" s="6" t="s">
-        <v>609</v>
+        <v>607</v>
       </c>
     </row>
     <row r="158" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A158" s="7" t="s">
-        <v>610</v>
+        <v>608</v>
       </c>
       <c r="B158" s="6" t="s">
-        <v>568</v>
+        <v>566</v>
       </c>
       <c r="C158" s="6" t="s">
-        <v>611</v>
+        <v>609</v>
       </c>
     </row>
     <row r="159" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A159" s="7" t="s">
-        <v>612</v>
+        <v>610</v>
       </c>
       <c r="B159" s="6" t="s">
-        <v>568</v>
+        <v>566</v>
       </c>
       <c r="C159" s="6" t="s">
-        <v>613</v>
+        <v>611</v>
       </c>
     </row>
     <row r="160" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A160" s="7" t="s">
-        <v>614</v>
+        <v>612</v>
       </c>
       <c r="B160" s="6" t="s">
-        <v>568</v>
+        <v>566</v>
       </c>
       <c r="C160" s="6" t="s">
-        <v>615</v>
+        <v>613</v>
       </c>
     </row>
     <row r="161" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A161" s="7" t="s">
-        <v>616</v>
+        <v>614</v>
       </c>
       <c r="B161" s="6" t="s">
-        <v>568</v>
+        <v>566</v>
       </c>
       <c r="C161" s="6" t="s">
-        <v>617</v>
+        <v>615</v>
       </c>
     </row>
     <row r="162" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A162" s="7" t="s">
+        <v>616</v>
+      </c>
+      <c r="B162" s="6" t="s">
+        <v>617</v>
+      </c>
+      <c r="C162" s="6" t="s">
         <v>618</v>
-      </c>
-      <c r="B162" s="6" t="s">
-        <v>619</v>
-      </c>
-      <c r="C162" s="6" t="s">
-        <v>620</v>
       </c>
     </row>
     <row r="163" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A163" s="7" t="s">
-        <v>621</v>
+        <v>619</v>
       </c>
       <c r="B163" s="6" t="s">
-        <v>619</v>
+        <v>617</v>
       </c>
       <c r="C163" s="6" t="s">
-        <v>622</v>
+        <v>620</v>
       </c>
     </row>
     <row r="164" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A164" s="7" t="s">
-        <v>623</v>
+        <v>621</v>
       </c>
       <c r="B164" s="6" t="s">
-        <v>619</v>
+        <v>617</v>
       </c>
       <c r="C164" s="6" t="s">
-        <v>624</v>
+        <v>622</v>
       </c>
     </row>
     <row r="165" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A165" s="7" t="s">
-        <v>625</v>
+        <v>623</v>
       </c>
       <c r="B165" s="6" t="s">
-        <v>619</v>
+        <v>617</v>
       </c>
       <c r="C165" s="6" t="s">
-        <v>626</v>
+        <v>624</v>
       </c>
     </row>
     <row r="166" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A166" s="7" t="s">
-        <v>627</v>
+        <v>625</v>
       </c>
       <c r="B166" s="6" t="s">
-        <v>619</v>
+        <v>617</v>
       </c>
       <c r="C166" s="6" t="s">
-        <v>628</v>
+        <v>626</v>
       </c>
     </row>
     <row r="167" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A167" s="7" t="s">
-        <v>629</v>
+        <v>627</v>
       </c>
       <c r="B167" s="6" t="s">
-        <v>619</v>
+        <v>617</v>
       </c>
       <c r="C167" s="6" t="s">
-        <v>630</v>
+        <v>628</v>
       </c>
     </row>
     <row r="168" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A168" s="7" t="s">
-        <v>631</v>
+        <v>629</v>
       </c>
       <c r="B168" s="6" t="s">
-        <v>619</v>
+        <v>617</v>
       </c>
       <c r="C168" s="6" t="s">
-        <v>632</v>
+        <v>630</v>
       </c>
     </row>
     <row r="169" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A169" s="7" t="s">
-        <v>633</v>
+        <v>631</v>
       </c>
       <c r="B169" s="6" t="s">
-        <v>619</v>
+        <v>617</v>
       </c>
       <c r="C169" s="6" t="s">
-        <v>634</v>
+        <v>632</v>
       </c>
     </row>
     <row r="170" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A170" s="7" t="s">
-        <v>635</v>
+        <v>633</v>
       </c>
       <c r="B170" s="6" t="s">
-        <v>619</v>
+        <v>617</v>
       </c>
       <c r="C170" s="6" t="s">
-        <v>636</v>
+        <v>634</v>
       </c>
     </row>
     <row r="171" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A171" s="7" t="s">
-        <v>637</v>
+        <v>635</v>
       </c>
       <c r="B171" s="6" t="s">
-        <v>619</v>
+        <v>617</v>
       </c>
       <c r="C171" s="6" t="s">
-        <v>638</v>
+        <v>636</v>
       </c>
     </row>
     <row r="172" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A172" s="7" t="s">
+        <v>637</v>
+      </c>
+      <c r="B172" s="6" t="s">
+        <v>638</v>
+      </c>
+      <c r="C172" s="6" t="s">
         <v>639</v>
-      </c>
-      <c r="B172" s="6" t="s">
-        <v>640</v>
-      </c>
-      <c r="C172" s="6" t="s">
-        <v>641</v>
       </c>
     </row>
     <row r="173" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A173" s="7" t="s">
-        <v>642</v>
+        <v>640</v>
       </c>
       <c r="B173" s="6" t="s">
-        <v>640</v>
+        <v>638</v>
       </c>
       <c r="C173" s="6" t="s">
-        <v>643</v>
+        <v>641</v>
       </c>
     </row>
     <row r="174" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A174" s="7" t="s">
-        <v>644</v>
+        <v>642</v>
       </c>
       <c r="B174" s="6" t="s">
-        <v>640</v>
+        <v>638</v>
       </c>
       <c r="C174" s="6" t="s">
-        <v>645</v>
+        <v>643</v>
       </c>
     </row>
     <row r="175" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A175" s="7" t="s">
-        <v>646</v>
+        <v>644</v>
       </c>
       <c r="B175" s="6" t="s">
-        <v>640</v>
+        <v>638</v>
       </c>
       <c r="C175" s="6" t="s">
-        <v>647</v>
+        <v>645</v>
       </c>
     </row>
     <row r="176" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A176" s="7" t="s">
-        <v>648</v>
+        <v>646</v>
       </c>
       <c r="B176" s="6" t="s">
-        <v>640</v>
+        <v>638</v>
       </c>
       <c r="C176" s="6" t="s">
-        <v>649</v>
+        <v>647</v>
       </c>
     </row>
     <row r="177" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A177" s="7" t="s">
-        <v>650</v>
+        <v>648</v>
       </c>
       <c r="B177" s="6" t="s">
-        <v>640</v>
+        <v>638</v>
       </c>
       <c r="C177" s="6" t="s">
-        <v>651</v>
+        <v>649</v>
       </c>
     </row>
     <row r="178" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A178" s="7" t="s">
-        <v>652</v>
+        <v>650</v>
       </c>
       <c r="B178" s="6" t="s">
-        <v>640</v>
+        <v>638</v>
       </c>
       <c r="C178" s="6" t="s">
-        <v>653</v>
+        <v>651</v>
       </c>
     </row>
     <row r="179" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A179" s="7" t="s">
-        <v>654</v>
+        <v>652</v>
       </c>
       <c r="B179" s="6" t="s">
-        <v>640</v>
+        <v>638</v>
       </c>
       <c r="C179" s="6" t="s">
-        <v>655</v>
+        <v>653</v>
       </c>
     </row>
     <row r="180" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A180" s="7" t="s">
-        <v>656</v>
+        <v>654</v>
       </c>
       <c r="B180" s="6" t="s">
-        <v>640</v>
+        <v>638</v>
       </c>
       <c r="C180" s="6" t="s">
-        <v>657</v>
+        <v>655</v>
       </c>
     </row>
     <row r="181" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A181" s="7" t="s">
+        <v>656</v>
+      </c>
+      <c r="B181" s="6" t="s">
+        <v>657</v>
+      </c>
+      <c r="C181" s="6" t="s">
         <v>658</v>
-      </c>
-      <c r="B181" s="6" t="s">
-        <v>659</v>
-      </c>
-      <c r="C181" s="6" t="s">
-        <v>660</v>
       </c>
     </row>
     <row r="182" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A182" s="7" t="s">
-        <v>661</v>
+        <v>659</v>
       </c>
       <c r="B182" s="6" t="s">
-        <v>659</v>
+        <v>657</v>
       </c>
       <c r="C182" s="6" t="s">
-        <v>662</v>
+        <v>660</v>
       </c>
     </row>
     <row r="183" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A183" s="7" t="s">
-        <v>663</v>
+        <v>661</v>
       </c>
       <c r="B183" s="6" t="s">
-        <v>659</v>
+        <v>657</v>
       </c>
       <c r="C183" s="6" t="s">
-        <v>664</v>
+        <v>662</v>
       </c>
     </row>
     <row r="184" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A184" s="7" t="s">
-        <v>665</v>
+        <v>663</v>
       </c>
       <c r="B184" s="6" t="s">
-        <v>659</v>
+        <v>657</v>
       </c>
       <c r="C184" s="6" t="s">
-        <v>666</v>
+        <v>664</v>
       </c>
     </row>
     <row r="185" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A185" s="7" t="s">
-        <v>667</v>
+        <v>665</v>
       </c>
       <c r="B185" s="6" t="s">
-        <v>659</v>
+        <v>657</v>
       </c>
       <c r="C185" s="6" t="s">
-        <v>668</v>
+        <v>666</v>
       </c>
     </row>
     <row r="186" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A186" s="7" t="s">
-        <v>669</v>
+        <v>667</v>
       </c>
       <c r="B186" s="6" t="s">
-        <v>659</v>
+        <v>657</v>
       </c>
       <c r="C186" s="6" t="s">
-        <v>670</v>
+        <v>668</v>
       </c>
     </row>
     <row r="187" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A187" s="7" t="s">
-        <v>671</v>
+        <v>669</v>
       </c>
       <c r="B187" s="6" t="s">
-        <v>659</v>
+        <v>657</v>
       </c>
       <c r="C187" s="6" t="s">
-        <v>672</v>
+        <v>670</v>
       </c>
     </row>
     <row r="188" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A188" s="7" t="s">
-        <v>673</v>
+        <v>671</v>
       </c>
       <c r="B188" s="6" t="s">
-        <v>659</v>
+        <v>657</v>
       </c>
       <c r="C188" s="6" t="s">
-        <v>674</v>
+        <v>672</v>
       </c>
     </row>
     <row r="189" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A189" s="7" t="s">
-        <v>675</v>
+        <v>673</v>
       </c>
       <c r="B189" s="6" t="s">
-        <v>659</v>
+        <v>657</v>
       </c>
       <c r="C189" s="6" t="s">
-        <v>676</v>
+        <v>674</v>
       </c>
     </row>
     <row r="190" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A190" s="7" t="s">
-        <v>677</v>
+        <v>675</v>
       </c>
       <c r="B190" s="6" t="s">
-        <v>659</v>
+        <v>657</v>
       </c>
       <c r="C190" s="6" t="s">
-        <v>678</v>
+        <v>676</v>
       </c>
     </row>
     <row r="191" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A191" s="7" t="s">
-        <v>679</v>
+        <v>677</v>
       </c>
       <c r="B191" s="6" t="s">
-        <v>659</v>
+        <v>657</v>
       </c>
       <c r="C191" s="6" t="s">
-        <v>680</v>
+        <v>678</v>
       </c>
     </row>
     <row r="192" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A192" s="7" t="s">
-        <v>681</v>
+        <v>679</v>
       </c>
       <c r="B192" s="6" t="s">
-        <v>659</v>
+        <v>657</v>
       </c>
       <c r="C192" s="6" t="s">
-        <v>682</v>
+        <v>680</v>
       </c>
     </row>
     <row r="193" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A193" s="7" t="s">
+        <v>681</v>
+      </c>
+      <c r="B193" s="6" t="s">
+        <v>682</v>
+      </c>
+      <c r="C193" s="6" t="s">
         <v>683</v>
-      </c>
-      <c r="B193" s="6" t="s">
-        <v>684</v>
-      </c>
-      <c r="C193" s="6" t="s">
-        <v>685</v>
       </c>
     </row>
     <row r="194" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A194" s="7" t="s">
-        <v>686</v>
+        <v>684</v>
       </c>
       <c r="B194" s="6" t="s">
-        <v>684</v>
+        <v>682</v>
       </c>
       <c r="C194" s="6" t="s">
-        <v>687</v>
+        <v>685</v>
       </c>
     </row>
     <row r="195" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A195" s="7" t="s">
-        <v>688</v>
+        <v>686</v>
       </c>
       <c r="B195" s="6" t="s">
-        <v>684</v>
+        <v>682</v>
       </c>
       <c r="C195" s="6" t="s">
-        <v>689</v>
+        <v>687</v>
       </c>
     </row>
     <row r="196" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A196" s="7" t="s">
-        <v>690</v>
+        <v>688</v>
       </c>
       <c r="B196" s="6" t="s">
-        <v>684</v>
+        <v>682</v>
       </c>
       <c r="C196" s="6" t="s">
-        <v>691</v>
+        <v>689</v>
       </c>
     </row>
     <row r="197" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A197" s="7" t="s">
-        <v>692</v>
+        <v>690</v>
       </c>
       <c r="B197" s="6" t="s">
-        <v>684</v>
+        <v>682</v>
       </c>
       <c r="C197" s="6" t="s">
-        <v>693</v>
+        <v>691</v>
       </c>
     </row>
     <row r="198" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A198" s="7" t="s">
-        <v>694</v>
+        <v>692</v>
       </c>
       <c r="B198" s="6" t="s">
-        <v>684</v>
+        <v>682</v>
       </c>
       <c r="C198" s="6" t="s">
-        <v>695</v>
+        <v>693</v>
       </c>
     </row>
     <row r="199" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A199" s="7" t="s">
-        <v>696</v>
+        <v>694</v>
       </c>
       <c r="B199" s="6" t="s">
-        <v>684</v>
+        <v>682</v>
       </c>
       <c r="C199" s="6" t="s">
-        <v>697</v>
+        <v>695</v>
       </c>
     </row>
     <row r="200" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A200" s="7" t="s">
-        <v>698</v>
+        <v>696</v>
       </c>
       <c r="B200" s="6" t="s">
-        <v>684</v>
+        <v>682</v>
       </c>
       <c r="C200" s="6" t="s">
-        <v>699</v>
+        <v>697</v>
       </c>
     </row>
     <row r="201" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A201" s="7" t="s">
-        <v>700</v>
+        <v>698</v>
       </c>
       <c r="B201" s="6" t="s">
-        <v>684</v>
+        <v>682</v>
       </c>
       <c r="C201" s="6" t="s">
-        <v>701</v>
+        <v>699</v>
       </c>
     </row>
     <row r="202" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A202" s="7" t="s">
-        <v>702</v>
+        <v>700</v>
       </c>
       <c r="B202" s="6" t="s">
-        <v>684</v>
+        <v>682</v>
       </c>
       <c r="C202" s="6" t="s">
-        <v>703</v>
+        <v>701</v>
       </c>
     </row>
     <row r="203" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A203" s="7" t="s">
-        <v>704</v>
+        <v>702</v>
       </c>
       <c r="B203" s="6" t="s">
-        <v>684</v>
+        <v>682</v>
       </c>
       <c r="C203" s="6" t="s">
-        <v>705</v>
+        <v>703</v>
       </c>
     </row>
     <row r="204" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A204" s="7" t="s">
-        <v>706</v>
+        <v>704</v>
       </c>
       <c r="B204" s="6" t="s">
-        <v>684</v>
+        <v>682</v>
       </c>
       <c r="C204" s="6" t="s">
-        <v>707</v>
+        <v>705</v>
       </c>
     </row>
     <row r="205" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A205" s="7" t="s">
-        <v>708</v>
+        <v>706</v>
       </c>
       <c r="B205" s="6" t="s">
-        <v>684</v>
+        <v>682</v>
       </c>
       <c r="C205" s="6" t="s">
-        <v>709</v>
+        <v>707</v>
       </c>
     </row>
     <row r="206" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A206" s="7" t="s">
-        <v>710</v>
+        <v>708</v>
       </c>
       <c r="B206" s="6" t="s">
-        <v>684</v>
+        <v>682</v>
       </c>
       <c r="C206" s="6" t="s">
-        <v>711</v>
+        <v>709</v>
       </c>
     </row>
     <row r="207" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A207" s="7" t="s">
-        <v>712</v>
+        <v>710</v>
       </c>
       <c r="B207" s="6" t="s">
-        <v>684</v>
+        <v>682</v>
       </c>
       <c r="C207" s="6" t="s">
-        <v>713</v>
+        <v>711</v>
       </c>
     </row>
     <row r="208" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A208" s="7" t="s">
-        <v>714</v>
+        <v>712</v>
       </c>
       <c r="B208" s="6" t="s">
-        <v>684</v>
+        <v>682</v>
       </c>
       <c r="C208" s="6" t="s">
-        <v>715</v>
+        <v>713</v>
       </c>
     </row>
     <row r="209" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A209" s="7" t="s">
-        <v>716</v>
+        <v>714</v>
       </c>
       <c r="B209" s="6" t="s">
-        <v>684</v>
+        <v>682</v>
       </c>
       <c r="C209" s="6" t="s">
-        <v>717</v>
+        <v>715</v>
       </c>
     </row>
     <row r="210" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A210" s="7" t="s">
+        <v>716</v>
+      </c>
+      <c r="B210" s="6" t="s">
+        <v>717</v>
+      </c>
+      <c r="C210" s="6" t="s">
         <v>718</v>
-      </c>
-      <c r="B210" s="6" t="s">
-        <v>719</v>
-      </c>
-      <c r="C210" s="6" t="s">
-        <v>720</v>
       </c>
     </row>
     <row r="211" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A211" s="7" t="s">
-        <v>721</v>
+        <v>719</v>
       </c>
       <c r="B211" s="6" t="s">
-        <v>719</v>
+        <v>717</v>
       </c>
       <c r="C211" s="6" t="s">
-        <v>722</v>
+        <v>720</v>
       </c>
     </row>
     <row r="212" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A212" s="7" t="s">
-        <v>723</v>
+        <v>721</v>
       </c>
       <c r="B212" s="6" t="s">
-        <v>719</v>
+        <v>717</v>
       </c>
       <c r="C212" s="6" t="s">
-        <v>724</v>
+        <v>722</v>
       </c>
     </row>
     <row r="213" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A213" s="7" t="s">
-        <v>725</v>
+        <v>723</v>
       </c>
       <c r="B213" s="6" t="s">
-        <v>719</v>
+        <v>717</v>
       </c>
       <c r="C213" s="6" t="s">
-        <v>726</v>
+        <v>724</v>
       </c>
     </row>
     <row r="214" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A214" s="7" t="s">
-        <v>727</v>
+        <v>725</v>
       </c>
       <c r="B214" s="6" t="s">
-        <v>719</v>
+        <v>717</v>
       </c>
       <c r="C214" s="6" t="s">
-        <v>728</v>
+        <v>726</v>
       </c>
     </row>
     <row r="215" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A215" s="7" t="s">
+        <v>727</v>
+      </c>
+      <c r="B215" s="6" t="s">
+        <v>728</v>
+      </c>
+      <c r="C215" s="6" t="s">
         <v>729</v>
-      </c>
-      <c r="B215" s="6" t="s">
-        <v>730</v>
-      </c>
-      <c r="C215" s="6" t="s">
-        <v>731</v>
       </c>
     </row>
     <row r="216" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A216" s="7" t="s">
-        <v>732</v>
+        <v>730</v>
       </c>
       <c r="B216" s="6" t="s">
-        <v>730</v>
+        <v>728</v>
       </c>
       <c r="C216" s="6" t="s">
-        <v>733</v>
+        <v>731</v>
       </c>
     </row>
     <row r="217" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A217" s="7" t="s">
-        <v>734</v>
+        <v>732</v>
       </c>
       <c r="B217" s="6" t="s">
-        <v>730</v>
+        <v>728</v>
       </c>
       <c r="C217" s="6" t="s">
-        <v>735</v>
+        <v>733</v>
       </c>
     </row>
     <row r="218" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A218" s="7" t="s">
-        <v>736</v>
+        <v>734</v>
       </c>
       <c r="B218" s="6" t="s">
-        <v>730</v>
+        <v>728</v>
       </c>
       <c r="C218" s="6" t="s">
-        <v>737</v>
+        <v>735</v>
       </c>
     </row>
     <row r="219" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A219" s="7" t="s">
-        <v>738</v>
+        <v>736</v>
       </c>
       <c r="B219" s="6" t="s">
-        <v>730</v>
+        <v>728</v>
       </c>
       <c r="C219" s="6" t="s">
-        <v>739</v>
+        <v>737</v>
       </c>
     </row>
     <row r="220" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A220" s="7" t="s">
-        <v>740</v>
+        <v>738</v>
       </c>
       <c r="B220" s="6" t="s">
-        <v>730</v>
+        <v>728</v>
       </c>
       <c r="C220" s="6" t="s">
-        <v>741</v>
+        <v>739</v>
       </c>
     </row>
     <row r="221" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A221" s="7" t="s">
-        <v>742</v>
+        <v>740</v>
       </c>
       <c r="B221" s="6" t="s">
-        <v>730</v>
+        <v>728</v>
       </c>
       <c r="C221" s="6" t="s">
-        <v>743</v>
+        <v>741</v>
       </c>
     </row>
   </sheetData>
@@ -8722,8 +8724,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D104"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B71" workbookViewId="0">
-      <selection activeCell="C72" sqref="C72"/>
+    <sheetView tabSelected="1" topLeftCell="A81" workbookViewId="0">
+      <selection activeCell="A81" sqref="A81"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.3"/>
@@ -8735,24 +8737,24 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
+        <v>186</v>
+      </c>
+      <c r="B1" s="4" t="s">
         <v>187</v>
       </c>
-      <c r="B1" s="4" t="s">
-        <v>188</v>
-      </c>
       <c r="C1" s="5" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="304.5" x14ac:dyDescent="0.3">
       <c r="A2" s="9" t="s">
-        <v>746</v>
+        <v>744</v>
       </c>
       <c r="B2" s="9" t="s">
-        <v>744</v>
+        <v>742</v>
       </c>
       <c r="C2" s="9" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="409.5" x14ac:dyDescent="0.3">
@@ -8760,10 +8762,10 @@
         <v>0</v>
       </c>
       <c r="B3" s="9" t="s">
-        <v>745</v>
+        <v>743</v>
       </c>
       <c r="C3" s="9" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="377" x14ac:dyDescent="0.3">
@@ -8771,7 +8773,7 @@
         <v>1</v>
       </c>
       <c r="B4" s="9" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="C4" s="9" t="s">
         <v>2</v>
@@ -8782,10 +8784,10 @@
         <v>3</v>
       </c>
       <c r="B5" s="9" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="C5" s="9" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="362.5" x14ac:dyDescent="0.3">
@@ -8793,7 +8795,7 @@
         <v>4</v>
       </c>
       <c r="B6" s="9" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="C6" s="9" t="s">
         <v>5</v>
@@ -8804,7 +8806,7 @@
         <v>6</v>
       </c>
       <c r="B7" s="9" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="C7" s="9" t="s">
         <v>7</v>
@@ -8815,10 +8817,10 @@
         <v>8</v>
       </c>
       <c r="B8" s="9" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="C8" s="9" t="s">
-        <v>747</v>
+        <v>745</v>
       </c>
     </row>
     <row r="9" spans="1:3" ht="246.5" x14ac:dyDescent="0.3">
@@ -8826,10 +8828,10 @@
         <v>9</v>
       </c>
       <c r="B9" s="9" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="C9" s="9" t="s">
-        <v>756</v>
+        <v>754</v>
       </c>
     </row>
     <row r="10" spans="1:3" ht="409.5" x14ac:dyDescent="0.3">
@@ -8837,7 +8839,7 @@
         <v>10</v>
       </c>
       <c r="B10" s="9" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="C10" s="9" t="s">
         <v>11</v>
@@ -8848,7 +8850,7 @@
         <v>12</v>
       </c>
       <c r="B11" s="9" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="C11" s="9" t="s">
         <v>13</v>
@@ -8859,7 +8861,7 @@
         <v>14</v>
       </c>
       <c r="B12" s="9" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="C12" s="9" t="s">
         <v>15</v>
@@ -8870,7 +8872,7 @@
         <v>16</v>
       </c>
       <c r="B13" s="9" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="C13" s="9" t="s">
         <v>17</v>
@@ -8881,7 +8883,7 @@
         <v>18</v>
       </c>
       <c r="B14" s="9" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="C14" s="9" t="s">
         <v>19</v>
@@ -8892,7 +8894,7 @@
         <v>20</v>
       </c>
       <c r="B15" s="9" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="C15" s="9" t="s">
         <v>21</v>
@@ -8903,7 +8905,7 @@
         <v>22</v>
       </c>
       <c r="B16" s="9" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="C16" s="9" t="s">
         <v>23</v>
@@ -8914,10 +8916,10 @@
         <v>24</v>
       </c>
       <c r="B17" s="9" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="C17" s="9" t="s">
-        <v>748</v>
+        <v>746</v>
       </c>
     </row>
     <row r="18" spans="1:4" ht="145" x14ac:dyDescent="0.3">
@@ -8925,10 +8927,10 @@
         <v>25</v>
       </c>
       <c r="B18" s="9" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="C18" s="10" t="s">
-        <v>749</v>
+        <v>747</v>
       </c>
     </row>
     <row r="19" spans="1:4" ht="409.5" x14ac:dyDescent="0.3">
@@ -8936,7 +8938,7 @@
         <v>26</v>
       </c>
       <c r="B19" s="9" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="C19" s="9" t="s">
         <v>27</v>
@@ -8948,7 +8950,7 @@
         <v>28</v>
       </c>
       <c r="B20" s="9" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="C20" s="9" t="s">
         <v>29</v>
@@ -8959,7 +8961,7 @@
         <v>30</v>
       </c>
       <c r="B21" s="9" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="C21" s="9" t="s">
         <v>31</v>
@@ -8970,7 +8972,7 @@
         <v>32</v>
       </c>
       <c r="B22" s="9" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="C22" s="9" t="s">
         <v>33</v>
@@ -8981,7 +8983,7 @@
         <v>34</v>
       </c>
       <c r="B23" s="9" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="C23" s="9" t="s">
         <v>35</v>
@@ -8992,7 +8994,7 @@
         <v>36</v>
       </c>
       <c r="B24" s="9" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="C24" s="9" t="s">
         <v>37</v>
@@ -9003,10 +9005,10 @@
         <v>38</v>
       </c>
       <c r="B25" s="9" t="s">
+        <v>209</v>
+      </c>
+      <c r="C25" s="9" t="s">
         <v>210</v>
-      </c>
-      <c r="C25" s="9" t="s">
-        <v>211</v>
       </c>
     </row>
     <row r="26" spans="1:4" ht="319" x14ac:dyDescent="0.3">
@@ -9014,7 +9016,7 @@
         <v>39</v>
       </c>
       <c r="B26" s="9" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="C26" s="9" t="s">
         <v>40</v>
@@ -9025,10 +9027,10 @@
         <v>41</v>
       </c>
       <c r="B27" s="9" t="s">
+        <v>212</v>
+      </c>
+      <c r="C27" s="9" t="s">
         <v>213</v>
-      </c>
-      <c r="C27" s="9" t="s">
-        <v>214</v>
       </c>
     </row>
     <row r="28" spans="1:4" ht="290" x14ac:dyDescent="0.3">
@@ -9036,7 +9038,7 @@
         <v>42</v>
       </c>
       <c r="B28" s="9" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="C28" s="9" t="s">
         <v>43</v>
@@ -9047,7 +9049,7 @@
         <v>44</v>
       </c>
       <c r="B29" s="9" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="C29" s="9" t="s">
         <v>45</v>
@@ -9058,7 +9060,7 @@
         <v>46</v>
       </c>
       <c r="B30" s="9" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="C30" s="9" t="s">
         <v>47</v>
@@ -9069,7 +9071,7 @@
         <v>48</v>
       </c>
       <c r="B31" s="9" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="C31" s="9" t="s">
         <v>49</v>
@@ -9080,7 +9082,7 @@
         <v>50</v>
       </c>
       <c r="B32" s="9" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="C32" s="9" t="s">
         <v>51</v>
@@ -9091,10 +9093,10 @@
         <v>52</v>
       </c>
       <c r="B33" s="9" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="C33" s="9" t="s">
-        <v>749</v>
+        <v>747</v>
       </c>
     </row>
     <row r="34" spans="1:3" ht="217.5" x14ac:dyDescent="0.3">
@@ -9102,7 +9104,7 @@
         <v>53</v>
       </c>
       <c r="B34" s="9" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="C34" s="9" t="s">
         <v>54</v>
@@ -9113,7 +9115,7 @@
         <v>55</v>
       </c>
       <c r="B35" s="9" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="C35" s="9" t="s">
         <v>56</v>
@@ -9124,7 +9126,7 @@
         <v>57</v>
       </c>
       <c r="B36" s="9" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="C36" s="9" t="s">
         <v>58</v>
@@ -9135,7 +9137,7 @@
         <v>59</v>
       </c>
       <c r="B37" s="9" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="C37" s="9" t="s">
         <v>60</v>
@@ -9146,7 +9148,7 @@
         <v>61</v>
       </c>
       <c r="B38" s="9" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="C38" s="9" t="s">
         <v>62</v>
@@ -9157,10 +9159,10 @@
         <v>63</v>
       </c>
       <c r="B39" s="9" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="C39" s="9" t="s">
-        <v>750</v>
+        <v>748</v>
       </c>
     </row>
     <row r="40" spans="1:3" ht="409.5" x14ac:dyDescent="0.3">
@@ -9168,7 +9170,7 @@
         <v>64</v>
       </c>
       <c r="B40" s="9" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="C40" s="9" t="s">
         <v>65</v>
@@ -9179,7 +9181,7 @@
         <v>66</v>
       </c>
       <c r="B41" s="9" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="C41" s="9" t="s">
         <v>67</v>
@@ -9190,10 +9192,10 @@
         <v>68</v>
       </c>
       <c r="B42" s="9" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="C42" s="9" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
     </row>
     <row r="43" spans="1:3" ht="348" x14ac:dyDescent="0.3">
@@ -9201,7 +9203,7 @@
         <v>69</v>
       </c>
       <c r="B43" s="9" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="C43" s="9" t="s">
         <v>70</v>
@@ -9212,7 +9214,7 @@
         <v>71</v>
       </c>
       <c r="B44" s="9" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="C44" s="9" t="s">
         <v>72</v>
@@ -9223,7 +9225,7 @@
         <v>73</v>
       </c>
       <c r="B45" s="9" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="C45" s="9" t="s">
         <v>74</v>
@@ -9234,7 +9236,7 @@
         <v>75</v>
       </c>
       <c r="B46" s="9" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="C46" s="9" t="s">
         <v>76</v>
@@ -9245,7 +9247,7 @@
         <v>77</v>
       </c>
       <c r="B47" s="9" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="C47" s="9" t="s">
         <v>78</v>
@@ -9256,7 +9258,7 @@
         <v>79</v>
       </c>
       <c r="B48" s="9" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="C48" s="9" t="s">
         <v>80</v>
@@ -9267,7 +9269,7 @@
         <v>81</v>
       </c>
       <c r="B49" s="9" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="C49" s="9" t="s">
         <v>82</v>
@@ -9278,7 +9280,7 @@
         <v>83</v>
       </c>
       <c r="B50" s="9" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="C50" s="9" t="s">
         <v>84</v>
@@ -9289,7 +9291,7 @@
         <v>85</v>
       </c>
       <c r="B51" s="9" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="C51" s="9" t="s">
         <v>86</v>
@@ -9300,7 +9302,7 @@
         <v>87</v>
       </c>
       <c r="B52" s="9" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="C52" s="9" t="s">
         <v>88</v>
@@ -9311,10 +9313,10 @@
         <v>89</v>
       </c>
       <c r="B53" s="9" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="C53" s="9" t="s">
-        <v>751</v>
+        <v>749</v>
       </c>
     </row>
     <row r="54" spans="1:3" ht="409.5" x14ac:dyDescent="0.3">
@@ -9322,7 +9324,7 @@
         <v>90</v>
       </c>
       <c r="B54" s="9" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="C54" s="9" t="s">
         <v>91</v>
@@ -9333,7 +9335,7 @@
         <v>92</v>
       </c>
       <c r="B55" s="9" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="C55" s="9" t="s">
         <v>93</v>
@@ -9344,7 +9346,7 @@
         <v>94</v>
       </c>
       <c r="B56" s="9" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="C56" s="9" t="s">
         <v>95</v>
@@ -9355,7 +9357,7 @@
         <v>96</v>
       </c>
       <c r="B57" s="9" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="C57" s="9" t="s">
         <v>97</v>
@@ -9366,10 +9368,10 @@
         <v>98</v>
       </c>
       <c r="B58" s="9" t="s">
+        <v>244</v>
+      </c>
+      <c r="C58" s="9" t="s">
         <v>245</v>
-      </c>
-      <c r="C58" s="9" t="s">
-        <v>246</v>
       </c>
     </row>
     <row r="59" spans="1:3" ht="275.5" x14ac:dyDescent="0.3">
@@ -9377,7 +9379,7 @@
         <v>99</v>
       </c>
       <c r="B59" s="9" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="C59" s="9" t="s">
         <v>100</v>
@@ -9388,7 +9390,7 @@
         <v>101</v>
       </c>
       <c r="B60" s="9" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="C60" s="9" t="s">
         <v>102</v>
@@ -9399,7 +9401,7 @@
         <v>103</v>
       </c>
       <c r="B61" s="9" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="C61" s="9" t="s">
         <v>104</v>
@@ -9410,7 +9412,7 @@
         <v>105</v>
       </c>
       <c r="B62" s="9" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="C62" s="9" t="s">
         <v>106</v>
@@ -9432,7 +9434,7 @@
         <v>109</v>
       </c>
       <c r="B64" s="9" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="C64" s="9" t="s">
         <v>110</v>
@@ -9443,7 +9445,7 @@
         <v>111</v>
       </c>
       <c r="B65" s="9" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="C65" s="9" t="s">
         <v>112</v>
@@ -9454,7 +9456,7 @@
         <v>113</v>
       </c>
       <c r="B66" s="9" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="C66" s="9" t="s">
         <v>114</v>
@@ -9476,7 +9478,7 @@
         <v>117</v>
       </c>
       <c r="B68" s="9" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="C68" s="9" t="s">
         <v>118</v>
@@ -9487,7 +9489,7 @@
         <v>119</v>
       </c>
       <c r="B69" s="9" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="C69" s="9" t="s">
         <v>120</v>
@@ -9498,7 +9500,7 @@
         <v>121</v>
       </c>
       <c r="B70" s="9" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="C70" s="9" t="s">
         <v>122</v>
@@ -9509,10 +9511,10 @@
         <v>123</v>
       </c>
       <c r="B71" s="9" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="C71" s="9" t="s">
-        <v>757</v>
+        <v>755</v>
       </c>
     </row>
     <row r="72" spans="1:3" ht="217.5" x14ac:dyDescent="0.3">
@@ -9531,10 +9533,10 @@
         <v>126</v>
       </c>
       <c r="B73" s="9" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="C73" s="9" t="s">
-        <v>752</v>
+        <v>750</v>
       </c>
     </row>
     <row r="74" spans="1:3" ht="203" x14ac:dyDescent="0.3">
@@ -9542,7 +9544,7 @@
         <v>127</v>
       </c>
       <c r="B74" s="9" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="C74" s="9" t="s">
         <v>128</v>
@@ -9553,7 +9555,7 @@
         <v>129</v>
       </c>
       <c r="B75" s="9" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="C75" s="9" t="s">
         <v>130</v>
@@ -9564,7 +9566,7 @@
         <v>131</v>
       </c>
       <c r="B76" s="9" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="C76" s="9" t="s">
         <v>132</v>
@@ -9575,7 +9577,7 @@
         <v>133</v>
       </c>
       <c r="B77" s="9" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="C77" s="9" t="s">
         <v>134</v>
@@ -9586,7 +9588,7 @@
         <v>135</v>
       </c>
       <c r="B78" s="9" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="C78" s="9" t="s">
         <v>136</v>
@@ -9597,7 +9599,7 @@
         <v>137</v>
       </c>
       <c r="B79" s="9" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="C79" s="9" t="s">
         <v>138</v>
@@ -9608,7 +9610,7 @@
         <v>139</v>
       </c>
       <c r="B80" s="9" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="C80" s="9" t="s">
         <v>140</v>
@@ -9619,263 +9621,263 @@
         <v>141</v>
       </c>
       <c r="B81" s="9" t="s">
-        <v>266</v>
+        <v>756</v>
       </c>
       <c r="C81" s="9" t="s">
-        <v>142</v>
+        <v>757</v>
       </c>
     </row>
     <row r="82" spans="1:3" ht="217.5" x14ac:dyDescent="0.3">
       <c r="A82" s="9" t="s">
+        <v>142</v>
+      </c>
+      <c r="B82" s="9" t="s">
+        <v>265</v>
+      </c>
+      <c r="C82" s="9" t="s">
         <v>143</v>
-      </c>
-      <c r="B82" s="9" t="s">
-        <v>267</v>
-      </c>
-      <c r="C82" s="9" t="s">
-        <v>144</v>
       </c>
     </row>
     <row r="83" spans="1:3" ht="232" x14ac:dyDescent="0.3">
       <c r="A83" s="9" t="s">
+        <v>144</v>
+      </c>
+      <c r="B83" s="9" t="s">
+        <v>266</v>
+      </c>
+      <c r="C83" s="9" t="s">
         <v>145</v>
-      </c>
-      <c r="B83" s="9" t="s">
-        <v>268</v>
-      </c>
-      <c r="C83" s="9" t="s">
-        <v>146</v>
       </c>
     </row>
     <row r="84" spans="1:3" ht="275.5" x14ac:dyDescent="0.3">
       <c r="A84" s="9" t="s">
+        <v>146</v>
+      </c>
+      <c r="B84" s="9" t="s">
+        <v>267</v>
+      </c>
+      <c r="C84" s="9" t="s">
         <v>147</v>
-      </c>
-      <c r="B84" s="9" t="s">
-        <v>269</v>
-      </c>
-      <c r="C84" s="9" t="s">
-        <v>148</v>
       </c>
     </row>
     <row r="85" spans="1:3" ht="348" x14ac:dyDescent="0.3">
       <c r="A85" s="9" t="s">
+        <v>148</v>
+      </c>
+      <c r="B85" s="9" t="s">
+        <v>268</v>
+      </c>
+      <c r="C85" s="9" t="s">
         <v>149</v>
-      </c>
-      <c r="B85" s="9" t="s">
-        <v>270</v>
-      </c>
-      <c r="C85" s="9" t="s">
-        <v>150</v>
       </c>
     </row>
     <row r="86" spans="1:3" ht="290" x14ac:dyDescent="0.3">
       <c r="A86" s="9" t="s">
+        <v>150</v>
+      </c>
+      <c r="B86" s="9" t="s">
         <v>151</v>
       </c>
-      <c r="B86" s="9" t="s">
-        <v>152</v>
-      </c>
       <c r="C86" s="9" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="87" spans="1:3" ht="290" x14ac:dyDescent="0.3">
       <c r="A87" s="9" t="s">
+        <v>152</v>
+      </c>
+      <c r="B87" s="9" t="s">
         <v>153</v>
       </c>
-      <c r="B87" s="9" t="s">
-        <v>154</v>
-      </c>
       <c r="C87" s="9" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="88" spans="1:3" ht="348" x14ac:dyDescent="0.3">
       <c r="A88" s="9" t="s">
+        <v>154</v>
+      </c>
+      <c r="B88" s="9" t="s">
+        <v>269</v>
+      </c>
+      <c r="C88" s="9" t="s">
         <v>155</v>
-      </c>
-      <c r="B88" s="9" t="s">
-        <v>271</v>
-      </c>
-      <c r="C88" s="9" t="s">
-        <v>156</v>
       </c>
     </row>
     <row r="89" spans="1:3" ht="348" x14ac:dyDescent="0.3">
       <c r="A89" s="9" t="s">
+        <v>156</v>
+      </c>
+      <c r="B89" s="9" t="s">
         <v>157</v>
       </c>
-      <c r="B89" s="9" t="s">
-        <v>158</v>
-      </c>
       <c r="C89" s="9" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="90" spans="1:3" ht="246.5" x14ac:dyDescent="0.3">
       <c r="A90" s="9" t="s">
+        <v>158</v>
+      </c>
+      <c r="B90" s="9" t="s">
         <v>159</v>
       </c>
-      <c r="B90" s="9" t="s">
-        <v>160</v>
-      </c>
       <c r="C90" s="9" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="91" spans="1:3" ht="232" x14ac:dyDescent="0.3">
       <c r="A91" s="9" t="s">
+        <v>160</v>
+      </c>
+      <c r="B91" s="9" t="s">
         <v>161</v>
       </c>
-      <c r="B91" s="9" t="s">
-        <v>162</v>
-      </c>
       <c r="C91" s="9" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="92" spans="1:3" ht="333.5" x14ac:dyDescent="0.3">
       <c r="A92" s="9" t="s">
+        <v>162</v>
+      </c>
+      <c r="B92" s="9" t="s">
+        <v>270</v>
+      </c>
+      <c r="C92" s="9" t="s">
         <v>163</v>
-      </c>
-      <c r="B92" s="9" t="s">
-        <v>272</v>
-      </c>
-      <c r="C92" s="9" t="s">
-        <v>164</v>
       </c>
     </row>
     <row r="93" spans="1:3" ht="217.5" x14ac:dyDescent="0.3">
       <c r="A93" s="9" t="s">
+        <v>164</v>
+      </c>
+      <c r="B93" s="9" t="s">
+        <v>271</v>
+      </c>
+      <c r="C93" s="9" t="s">
         <v>165</v>
-      </c>
-      <c r="B93" s="9" t="s">
-        <v>273</v>
-      </c>
-      <c r="C93" s="9" t="s">
-        <v>166</v>
       </c>
     </row>
     <row r="94" spans="1:3" ht="217.5" x14ac:dyDescent="0.3">
       <c r="A94" s="9" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="B94" s="9" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="C94" s="9" t="s">
-        <v>754</v>
+        <v>752</v>
       </c>
     </row>
     <row r="95" spans="1:3" ht="203" x14ac:dyDescent="0.3">
       <c r="A95" s="9" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B95" s="9" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="C95" s="9" t="s">
-        <v>753</v>
+        <v>751</v>
       </c>
     </row>
     <row r="96" spans="1:3" ht="246.5" x14ac:dyDescent="0.3">
       <c r="A96" s="9" t="s">
+        <v>168</v>
+      </c>
+      <c r="B96" s="9" t="s">
+        <v>274</v>
+      </c>
+      <c r="C96" s="9" t="s">
         <v>169</v>
-      </c>
-      <c r="B96" s="9" t="s">
-        <v>276</v>
-      </c>
-      <c r="C96" s="9" t="s">
-        <v>170</v>
       </c>
     </row>
     <row r="97" spans="1:3" ht="333.5" x14ac:dyDescent="0.3">
       <c r="A97" s="9" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="B97" s="9" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="C97" s="9" t="s">
-        <v>755</v>
+        <v>753</v>
       </c>
     </row>
     <row r="98" spans="1:3" ht="333.5" x14ac:dyDescent="0.3">
       <c r="A98" s="9" t="s">
+        <v>171</v>
+      </c>
+      <c r="B98" s="9" t="s">
         <v>172</v>
       </c>
-      <c r="B98" s="9" t="s">
-        <v>173</v>
-      </c>
       <c r="C98" s="9" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
     </row>
     <row r="99" spans="1:3" ht="304.5" x14ac:dyDescent="0.3">
       <c r="A99" s="9" t="s">
+        <v>173</v>
+      </c>
+      <c r="B99" s="9" t="s">
+        <v>276</v>
+      </c>
+      <c r="C99" s="9" t="s">
         <v>174</v>
-      </c>
-      <c r="B99" s="9" t="s">
-        <v>278</v>
-      </c>
-      <c r="C99" s="9" t="s">
-        <v>175</v>
       </c>
     </row>
     <row r="100" spans="1:3" ht="290" x14ac:dyDescent="0.3">
       <c r="A100" s="9" t="s">
+        <v>175</v>
+      </c>
+      <c r="B100" s="9" t="s">
+        <v>277</v>
+      </c>
+      <c r="C100" s="9" t="s">
         <v>176</v>
-      </c>
-      <c r="B100" s="9" t="s">
-        <v>279</v>
-      </c>
-      <c r="C100" s="9" t="s">
-        <v>177</v>
       </c>
     </row>
     <row r="101" spans="1:3" ht="409.5" x14ac:dyDescent="0.3">
       <c r="A101" s="9" t="s">
+        <v>177</v>
+      </c>
+      <c r="B101" s="9" t="s">
+        <v>278</v>
+      </c>
+      <c r="C101" s="9" t="s">
         <v>178</v>
-      </c>
-      <c r="B101" s="9" t="s">
-        <v>280</v>
-      </c>
-      <c r="C101" s="9" t="s">
-        <v>179</v>
       </c>
     </row>
     <row r="102" spans="1:3" ht="159.5" x14ac:dyDescent="0.3">
       <c r="A102" s="9" t="s">
+        <v>179</v>
+      </c>
+      <c r="B102" s="9" t="s">
+        <v>279</v>
+      </c>
+      <c r="C102" s="9" t="s">
         <v>180</v>
-      </c>
-      <c r="B102" s="9" t="s">
-        <v>281</v>
-      </c>
-      <c r="C102" s="9" t="s">
-        <v>181</v>
       </c>
     </row>
     <row r="103" spans="1:3" ht="409.5" x14ac:dyDescent="0.3">
       <c r="A103" s="9" t="s">
+        <v>181</v>
+      </c>
+      <c r="B103" s="9" t="s">
+        <v>280</v>
+      </c>
+      <c r="C103" s="9" t="s">
         <v>182</v>
-      </c>
-      <c r="B103" s="9" t="s">
-        <v>282</v>
-      </c>
-      <c r="C103" s="9" t="s">
-        <v>183</v>
       </c>
     </row>
     <row r="104" spans="1:3" ht="391.5" x14ac:dyDescent="0.3">
       <c r="A104" s="9" t="s">
+        <v>183</v>
+      </c>
+      <c r="B104" s="9" t="s">
+        <v>281</v>
+      </c>
+      <c r="C104" s="9" t="s">
         <v>184</v>
-      </c>
-      <c r="B104" s="9" t="s">
-        <v>283</v>
-      </c>
-      <c r="C104" s="9" t="s">
-        <v>185</v>
       </c>
     </row>
   </sheetData>

</xml_diff>